<commit_message>
Histogram slider updated. Sri pilot graph changed
Histogram slider now supports arrow key use once secondary slider hits
bottom or top of histogram. Sri's excel pilot data graphed.
</commit_message>
<xml_diff>
--- a/FilmFinder/FilmFinder/bin/Release/Subject 2.xlsx
+++ b/FilmFinder/FilmFinder/bin/Release/Subject 2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="10">
   <si>
     <t>Actor</t>
   </si>
@@ -23,6 +23,27 @@
   </si>
   <si>
     <t>Director</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>multi</t>
+  </si>
+  <si>
+    <t>trackbar</t>
+  </si>
+  <si>
+    <t>histo</t>
+  </si>
+  <si>
+    <t>list1</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>mousewh</t>
   </si>
 </sst>
 </file>
@@ -507,7 +528,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
@@ -562,6 +584,523 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Subject 2'!$H$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>alpha</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>multi</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>trackbar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>histo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>list1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>active</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mousewh</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Subject 2'!$H$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>23148.777777777777</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37986.333333333336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20282.888888888891</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42963.111111111109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31915.777777777777</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31563.555555555555</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36976.666666666664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="43233280"/>
+        <c:axId val="43234816"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="43233280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43234816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43234816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43233280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Subject 2'!$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Subject 2'!$I$7:$I$13</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>alpha</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>multi</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>trackbar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>histo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>list1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>active</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mousewh</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Subject 2'!$J$7:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>31899.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26580.333333333332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27614</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76711</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41551.333333333336</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57462.666666666664</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64906.666666666664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Subject 2'!$K$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actress</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Subject 2'!$I$7:$I$13</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>alpha</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>multi</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>trackbar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>histo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>list1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>active</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mousewh</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Subject 2'!$K$7:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>24750</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45486.333333333336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18118</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18303.333333333332</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37549</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12805</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25986</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Subject 2'!$L$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Director</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Subject 2'!$I$7:$I$13</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>alpha</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>multi</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>trackbar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>histo</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>list1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>active</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mousewh</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Subject 2'!$L$7:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>12796.666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41892.333333333336</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15116.666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16647</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24423</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20037.333333333332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="45665664"/>
+        <c:axId val="45667456"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="45665664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="45667456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="45667456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="45665664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -851,13 +1390,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:L13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -876,8 +1417,29 @@
       <c r="F1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -896,8 +1458,36 @@
       <c r="F2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>AVERAGE(E1:E9)</f>
+        <v>23148.777777777777</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(E10:E18)</f>
+        <v>37986.333333333336</v>
+      </c>
+      <c r="J2">
+        <f>AVERAGE(E19:E27)</f>
+        <v>20282.888888888891</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(E28:E36)</f>
+        <v>42963.111111111109</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(E37:E45)</f>
+        <v>31915.777777777777</v>
+      </c>
+      <c r="M2">
+        <f>AVERAGE(E46:E54)</f>
+        <v>31563.555555555555</v>
+      </c>
+      <c r="N2">
+        <f>AVERAGE(E55:E63)</f>
+        <v>36976.666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -917,7 +1507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -937,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -957,7 +1547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -976,8 +1566,18 @@
       <c r="F6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -996,8 +1596,23 @@
       <c r="F7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <f>AVERAGE(E1:E3)</f>
+        <v>31899.666666666668</v>
+      </c>
+      <c r="K7" s="1">
+        <f>AVERAGE(E4:E6)</f>
+        <v>24750</v>
+      </c>
+      <c r="L7" s="1">
+        <f>AVERAGE(E7:E9)</f>
+        <v>12796.666666666666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1016,8 +1631,23 @@
       <c r="F8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <f>AVERAGE(E10:E12)</f>
+        <v>26580.333333333332</v>
+      </c>
+      <c r="K8" s="1">
+        <f>AVERAGE(E13:E15)</f>
+        <v>45486.333333333336</v>
+      </c>
+      <c r="L8" s="1">
+        <f>AVERAGE(E16:E18)</f>
+        <v>41892.333333333336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1036,8 +1666,23 @@
       <c r="F9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <f>AVERAGE(E19:E21)</f>
+        <v>27614</v>
+      </c>
+      <c r="K9" s="1">
+        <f>AVERAGE(E22:E24)</f>
+        <v>18118</v>
+      </c>
+      <c r="L9" s="1">
+        <f>AVERAGE(E25:E27)</f>
+        <v>15116.666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1056,8 +1701,23 @@
       <c r="F10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="1">
+        <f>AVERAGE(E28:E30)</f>
+        <v>76711</v>
+      </c>
+      <c r="K10" s="1">
+        <f>AVERAGE(E31:E33)</f>
+        <v>18303.333333333332</v>
+      </c>
+      <c r="L10" s="1">
+        <f>AVERAGE(E34:E36)</f>
+        <v>33875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1076,8 +1736,23 @@
       <c r="F11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="1">
+        <f>AVERAGE(E37:E39)</f>
+        <v>41551.333333333336</v>
+      </c>
+      <c r="K11" s="1">
+        <f>AVERAGE(E40:E42)</f>
+        <v>37549</v>
+      </c>
+      <c r="L11" s="1">
+        <f>AVERAGE(E43:E45)</f>
+        <v>16647</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1096,8 +1771,23 @@
       <c r="F12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="1">
+        <f>AVERAGE(E46:E48)</f>
+        <v>57462.666666666664</v>
+      </c>
+      <c r="K12" s="1">
+        <f>AVERAGE(E49:E51)</f>
+        <v>12805</v>
+      </c>
+      <c r="L12" s="1">
+        <f>AVERAGE(E52:E54)</f>
+        <v>24423</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1116,8 +1806,23 @@
       <c r="F13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="1">
+        <f>AVERAGE(E55:E57)</f>
+        <v>64906.666666666664</v>
+      </c>
+      <c r="K13" s="1">
+        <f>AVERAGE(E58:E60)</f>
+        <v>25986</v>
+      </c>
+      <c r="L13" s="1">
+        <f>AVERAGE(E61:E63)</f>
+        <v>20037.333333333332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1137,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1157,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2119,5 +2824,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>